<commit_message>
Reset project to run Main.xaml and finished building Scrape test case with embedded email bodies
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Test_Framework/_Tests.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Test_Framework/_Tests.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B434C44-C38C-4F13-ABDB-169CCEDAAC46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="102">
   <si>
     <t>WorkflowFile</t>
   </si>
@@ -109,9 +110,6 @@
     <t>Is an error thrown if I try to navigate somewhere bad</t>
   </si>
   <si>
-    <t>Initialise config</t>
-  </si>
-  <si>
     <t>DEV</t>
   </si>
   <si>
@@ -154,15 +152,6 @@
     <t>\Test_Framework\Exchange\Test_GetExchangeMail.xaml</t>
   </si>
   <si>
-    <t>FA_Proforma_SSO_rpa00002,https://outlook.office365.com/EWS/Exchange.asmx,Inbox\Proforma - Dev\New,Inbox\Proforma - Dev,Inbox\Proforma - Dev\Error</t>
-  </si>
-  <si>
-    <t>FA_Proforma_SSO_rpa00002,https://outlook.office365.com/EWS/Exchange.asmx,contractandgrants@uq.edu.au\Inbox\Minion - GRL Proforma\Testing,contractandgrants@uq.edu.au\Inbox\Minion - GRL Proforma\Testing\New,contractandgrants@uq.edu.au\Inbox\Minion - GRL Proforma\Testing\Error</t>
-  </si>
-  <si>
-    <t>FA_Proforma_SSO_rpa00002,https://outlook.office365.com/EWS/Exchange.asmx,contractandgrants@uq.edu.au\Inbox\Minion - GRL Proforma\New,contractandgrants@uq.edu.au\Inbox\Minion - GRL Proforma\Error</t>
-  </si>
-  <si>
     <t>FA_Proforma_BadCredentials,https://outlook.office365.com/EWS/Exchange.asmx,contractandgrants@uq.edu.au\Inbox\Minion - GRL Proforma\Testing</t>
   </si>
   <si>
@@ -191,12 +180,259 @@
   </si>
   <si>
     <t>FA_Proforma_SSO_rpa00002,https://www.unifi.uq.edu.au/psp/ps/?cmd=login</t>
+  </si>
+  <si>
+    <t>Initialise with Staging Config</t>
+  </si>
+  <si>
+    <t>Initialise with Development Config</t>
+  </si>
+  <si>
+    <t>\Test_Framework\Test_InitAllSettings.xaml</t>
+  </si>
+  <si>
+    <t>FA_Proforma_SSO_rpa00002,https://outlook.office365.com/EWS/Exchange.asmx,Inbox\Proforma - Dev</t>
+  </si>
+  <si>
+    <t>FA_Proforma_SSO_rpa00002,https://outlook.office365.com/EWS/Exchange.asmx,contractandgrants@uq.edu.au\Inbox\Minion - GRL Proforma\Testing</t>
+  </si>
+  <si>
+    <t>FA_Proforma_SSO_rpa00002,https://outlook.office365.com/EWS/Exchange.asmx,contractandgrants@uq.edu.au\Inbox\Minion - GRL Proforma</t>
+  </si>
+  <si>
+    <t>OpUnit Fac</t>
+  </si>
+  <si>
+    <t>OpUnit Sch</t>
+  </si>
+  <si>
+    <t>OpUnit Sect</t>
+  </si>
+  <si>
+    <t>OpUnit Site</t>
+  </si>
+  <si>
+    <t>UndAcc Opal</t>
+  </si>
+  <si>
+    <t>UndAcc Site</t>
+  </si>
+  <si>
+    <t>UndAcc Fund</t>
+  </si>
+  <si>
+    <t>UndAcc Func</t>
+  </si>
+  <si>
+    <t>Empty Table</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Successful</t>
+  </si>
+  <si>
+    <t>Invalid Faculty Code in Operational Unit Code</t>
+  </si>
+  <si>
+    <t>Invalid Opal Code in Unerwriting Account</t>
+  </si>
+  <si>
+    <t>Invalid Site Code in Unerwriting Account</t>
+  </si>
+  <si>
+    <t>Invalid Fund Code in Unerwriting Account</t>
+  </si>
+  <si>
+    <t>Invalid Function Code in Unerwriting Account</t>
+  </si>
+  <si>
+    <t>Invalid Site Code in Operational Unit Code</t>
+  </si>
+  <si>
+    <t>Invalid Section Code in Operational Unit Code</t>
+  </si>
+  <si>
+    <t>Invalid School Code in Operational Unit Code</t>
+  </si>
+  <si>
+    <t>Valid proforma email without any fields populated</t>
+  </si>
+  <si>
+    <t>Email without any proforma content</t>
+  </si>
+  <si>
+    <t>Valid proforma email with all fields populated</t>
+  </si>
+  <si>
+    <t>Test_Framework\Exchange\Test_ScrapeEmail.xaml</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>No exception thrown</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>An exception was meant to be thrown</t>
+  </si>
+  <si>
+    <t>Should throw AppEx: UiPath.Mail.ExchangeException: The Autodiscover service couldn't be located._x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Should throw AppEx: Microsoft.Exchange.WebServices.Data.ServiceResponseException: The SMTP address has no mailbox associated with it._x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Should throw AppEx: System.Exception: Couldn't find Minion - Incorrect Path_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Should throw AppEx: System.Exception: Couldn't find Excess Mailbox Path_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Wasn't meant to throw AppEx: System.IO.FileNotFoundException: Could not find file 'C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Test_Framework\Test_LoginToUniFi.xaml'._x000D_
+File name: 'C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Test_Framework\Test_LoginToUniFi.xaml'_x000D_
+   at System.IO.__Error.WinIOError(Int32 errorCode, String maybeFullPath)_x000D_
+   at System.IO.FileStream.Init(String path, FileMode mode, FileAccess access, Int32 rights, Boolean useRights, FileShare share, Int32 bufferSize, FileOptions options, SECURITY_ATTRIBUTES secAttrs, String msgPath, Boolean bFromProxy, Boolean useLongPath, Boolean checkHost)_x000D_
+   at System.IO.FileStream..ctor(String path, FileMode mode, FileAccess access, FileShare share)_x000D_
+   at UiPath.Executor.WorkflowRuntime.GetWorkflowFileStream(String workflowFile) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 87_x000D_
+   at UiPath.Executor.WorkflowRuntime.Load(String workflowFile) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 74_x000D_
+   at UiPath.Executor.WorkflowRunner.BeginExecuteInProcess(AsyncCallback callback, TaskCompletionSource`1 taskCompletionSource) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 240_x000D_
+   at UiPath.Executor.WorkflowRunner.BeginExecute(AsyncCallback callback, Object state) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 184_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.BeginExecute(AsyncCodeActivityContext context, AsyncCallback callback, Object state)_x000D_
+   at System.Activities.AsyncCodeActivity.InternalExecute(ActivityInstance instance, ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   at System.Activities.ActivityInstance.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   at System.Activities.Runtime.ActivityExecutor.ExecuteActivityWorkItem.ExecuteBody(ActivityExecutor executor, BookmarkManager bookmarkManager, Location resultLocation)</t>
+  </si>
+  <si>
+    <t>Should throw AppEx: System.IO.FileNotFoundException: Could not find file 'C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Test_Framework\Test_NavToMenuItem.xaml'._x000D_
+File name: 'C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Test_Framework\Test_NavToMenuItem.xaml'_x000D_
+   at System.IO.__Error.WinIOError(Int32 errorCode, String maybeFullPath)_x000D_
+   at System.IO.FileStream.Init(String path, FileMode mode, FileAccess access, Int32 rights, Boolean useRights, FileShare share, Int32 bufferSize, FileOptions options, SECURITY_ATTRIBUTES secAttrs, String msgPath, Boolean bFromProxy, Boolean useLongPath, Boolean checkHost)_x000D_
+   at System.IO.FileStream..ctor(String path, FileMode mode, FileAccess access, FileShare share)_x000D_
+   at UiPath.Executor.WorkflowRuntime.GetWorkflowFileStream(String workflowFile) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 87_x000D_
+   at UiPath.Executor.WorkflowRuntime.Load(String workflowFile) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 74_x000D_
+   at UiPath.Executor.WorkflowRunner.BeginExecuteInProcess(AsyncCallback callback, TaskCompletionSource`1 taskCompletionSource) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 240_x000D_
+   at UiPath.Executor.WorkflowRunner.BeginExecute(AsyncCallback callback, Object state) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 184_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.BeginExecute(AsyncCodeActivityContext context, AsyncCallback callback, Object state)_x000D_
+   at System.Activities.AsyncCodeActivity.InternalExecute(ActivityInstance instance, ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   at System.Activities.ActivityInstance.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   at System.Activities.Runtime.ActivityExecutor.ExecuteActivityWorkItem.ExecuteBody(ActivityExecutor executor, BookmarkManager bookmarkManager, Location resultLocation)</t>
+  </si>
+  <si>
+    <t>Wasn't meant to throw AppEx: System.IO.FileNotFoundException: Could not find file 'C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Test_Framework\Test_NavToMenuItem.xaml'._x000D_
+File name: 'C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Test_Framework\Test_NavToMenuItem.xaml'_x000D_
+   at System.IO.__Error.WinIOError(Int32 errorCode, String maybeFullPath)_x000D_
+   at System.IO.FileStream.Init(String path, FileMode mode, FileAccess access, Int32 rights, Boolean useRights, FileShare share, Int32 bufferSize, FileOptions options, SECURITY_ATTRIBUTES secAttrs, String msgPath, Boolean bFromProxy, Boolean useLongPath, Boolean checkHost)_x000D_
+   at System.IO.FileStream..ctor(String path, FileMode mode, FileAccess access, FileShare share)_x000D_
+   at UiPath.Executor.WorkflowRuntime.GetWorkflowFileStream(String workflowFile) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 87_x000D_
+   at UiPath.Executor.WorkflowRuntime.Load(String workflowFile) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 74_x000D_
+   at UiPath.Executor.WorkflowRunner.BeginExecuteInProcess(AsyncCallback callback, TaskCompletionSource`1 taskCompletionSource) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 240_x000D_
+   at UiPath.Executor.WorkflowRunner.BeginExecute(AsyncCallback callback, Object state) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 184_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.BeginExecute(AsyncCodeActivityContext context, AsyncCallback callback, Object state)_x000D_
+   at System.Activities.AsyncCodeActivity.InternalExecute(ActivityInstance instance, ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   at System.Activities.ActivityInstance.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   at System.Activities.Runtime.ActivityExecutor.ExecuteActivityWorkItem.ExecuteBody(ActivityExecutor executor, BookmarkManager bookmarkManager, Location resultLocation)</t>
+  </si>
+  <si>
+    <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: RM Number ---&gt; UiPath.Core.Activities.ActivityTimeoutException: Activity timeout exceeded_x000D_
+   at UiPath.Core.Activities.WaitUiElementAppear.EndExecute(NativeActivityContext context, IAsyncResult result)_x000D_
+   at UiPath.Core.Activities.AsyncNativeActivity`1.BookmarkResumptionCallback(NativeActivityContext context, Bookmark bookmark, Object value)_x000D_
+   at System.Activities.Runtime.BookmarkCallbackWrapper.Invoke(NativeActivityContext context, Bookmark bookmark, Object value)_x000D_
+   at System.Activities.Runtime.BookmarkWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   --- End of inner exception stack trace ---_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Op Unit: Faculty, School, Section, Site &amp; Under Acc: Opal, Site, Fund, Function_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Op Unit: Faculty_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Op Unit: School_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Op Unit: Section_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Op Unit: Site_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Under Acc: Opal_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Under Acc: Site_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Under Acc: Fund_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Under Acc: Function_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -548,16 +784,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.5703125" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="64" customWidth="1"/>
@@ -589,22 +825,22 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -612,32 +848,32 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -649,7 +885,7 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -660,14 +896,14 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="5" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -675,13 +911,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
@@ -689,13 +925,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -703,72 +939,72 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -779,29 +1015,29 @@
         <v>3</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
@@ -815,7 +1051,7 @@
     </row>
     <row r="20" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -829,7 +1065,7 @@
     </row>
     <row r="23" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -840,7 +1076,7 @@
     </row>
     <row r="24" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -854,7 +1090,7 @@
     </row>
     <row r="25" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
@@ -868,7 +1104,7 @@
     </row>
     <row r="26" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
@@ -882,7 +1118,7 @@
     </row>
     <row r="27" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
         <v>21</v>
@@ -896,7 +1132,7 @@
     </row>
     <row r="28" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
@@ -906,9 +1142,169 @@
         <v>19</v>
       </c>
     </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D42"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31:B38 B2:B13 B23:B28 B17:B18 B19:B20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:B20 B2:B13 B23:B40" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Success,BRE,AppEx"</formula1>
     </dataValidation>
   </dataValidations>
@@ -918,11 +1314,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,55 +1348,554 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10"/>
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
       <c r="C10"/>
+      <c r="D10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="2"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="2"/>
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="5">
+        <v>2018001377</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="5">
+        <v>200000199</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="5">
+        <v>2018001812</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="5">
+        <v>201100215</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B30" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Success,BRE,AppEx"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Test scenarios roughly finished for all processes to assist in UiPath upgrade
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Test_Framework/_Tests.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Test_Framework/_Tests.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B434C44-C38C-4F13-ABDB-169CCEDAAC46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="109">
   <si>
     <t>WorkflowFile</t>
   </si>
@@ -95,9 +94,6 @@
     <t>Test_Framework\Test_InitAllSettings.xaml</t>
   </si>
   <si>
-    <t>\Test_Framework\Test_LoginToUniFi.xaml</t>
-  </si>
-  <si>
     <t>Grants\Proposals\Maintain Staged Proposals</t>
   </si>
   <si>
@@ -116,9 +112,6 @@
     <t>BAD</t>
   </si>
   <si>
-    <t>\Test_Framework\Test_SearchRMNumber.xaml</t>
-  </si>
-  <si>
     <t>Test_Framework\Exchange\Test_GetExchangeMail.xaml</t>
   </si>
   <si>
@@ -137,9 +130,6 @@
     <t>Check excess mailbox path</t>
   </si>
   <si>
-    <t>Test_Framework\Test_LoginToUniFi.xaml</t>
-  </si>
-  <si>
     <t>TEST</t>
   </si>
   <si>
@@ -176,9 +166,6 @@
     <t>Check UniFi Production login</t>
   </si>
   <si>
-    <t>Test_Framework\Test_NavToMenuItem.xaml</t>
-  </si>
-  <si>
     <t>FA_Proforma_SSO_rpa00002,https://www.unifi.uq.edu.au/psp/ps/?cmd=login</t>
   </si>
   <si>
@@ -281,77 +268,42 @@
     <t>An exception was meant to be thrown</t>
   </si>
   <si>
-    <t>Should throw AppEx: UiPath.Mail.ExchangeException: The Autodiscover service couldn't be located._x000D_
+    <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Under Acc: Function_x000D_
    at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
   <si>
-    <t>Should throw AppEx: Microsoft.Exchange.WebServices.Data.ServiceResponseException: The SMTP address has no mailbox associated with it._x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+    <t>Should throw AppEx: Microsoft.Exchange.WebServices.Data.ServiceRequestException: The request failed. The remote server returned an error: (503) Server Unavailable. ---&gt; System.Net.WebException: The remote server returned an error: (503) Server Unavailable._x000D_
+   at System.Net.HttpWebRequest.GetResponse()_x000D_
+   at Microsoft.Exchange.WebServices.Data.EwsHttpWebRequest.Microsoft.Exchange.WebServices.Data.IEwsHttpWebRequest.GetResponse() in \\REDMOND\EXCHANGE\BUILD\E15\15.00.0913.015\SOURCES\sources\dev\EwsManagedApi\src\EwsManagedApi\Core\EwsHttpWebRequest.cs:line 113_x000D_
+   at Microsoft.Exchange.WebServices.Data.ServiceRequestBase.GetEwsHttpWebResponse(IEwsHttpWebRequest request) in \\REDMOND\EXCHANGE\BUILD\E15\15.00.0913.015\SOURCES\sources\dev\EwsManagedApi\src\EwsManagedApi\Core\Requests\ServiceRequestBase.cs:line 821_x000D_
+   --- End of inner exception stack trace ---_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
   <si>
-    <t>Should throw AppEx: System.Exception: Couldn't find Minion - Incorrect Path_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+    <t>Should throw AppEx: Microsoft.Exchange.WebServices.Data.ServiceRequestException: The request failed. The remote name could not be resolved: 'invalid.office365.com' ---&gt; System.Net.WebException: The remote name could not be resolved: 'invalid.office365.com'_x000D_
+   at System.Net.HttpWebRequest.EndGetRequestStream(IAsyncResult asyncResult, TransportContext&amp; context)_x000D_
+   at System.Net.HttpWebRequest.EndGetRequestStream(IAsyncResult asyncResult)_x000D_
+   at Microsoft.Exchange.WebServices.Data.EwsHttpWebRequest.Microsoft.Exchange.WebServices.Data.IEwsHttpWebRequest.EndGetRequestStream(IAsyncResult asyncResult) in \\REDMOND\EXCHANGE\BUILD\E15\15.00.0913.015\SOURCES\sources\dev\EwsManagedApi\src\EwsManagedApi\Core\EwsHttpWebRequest.cs:line 79_x000D_
+   at Microsoft.Exchange.WebServices.Data.ServiceRequestBase.EmitRequest(IEwsHttpWebRequest request) in \\REDMOND\EXCHANGE\BUILD\E15\15.00.0913.015\SOURCES\sources\dev\EwsManagedApi\src\EwsManagedApi\Core\Requests\ServiceRequestBase.cs:line 413_x000D_
+   at Microsoft.Exchange.WebServices.Data.ServiceRequestBase.BuildEwsHttpWebRequest() in \\REDMOND\EXCHANGE\BUILD\E15\15.00.0913.015\SOURCES\sources\dev\EwsManagedApi\src\EwsManagedApi\Core\Requests\ServiceRequestBase.cs:line 790_x000D_
+   --- End of inner exception stack trace ---_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
   <si>
-    <t>Should throw AppEx: System.Exception: Couldn't find Excess Mailbox Path_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+    <t>Should throw AppEx: Microsoft.Exchange.WebServices.Data.ServiceResponseException: The SMTP address has no mailbox associated with it._x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
-  </si>
-  <si>
-    <t>Wasn't meant to throw AppEx: System.IO.FileNotFoundException: Could not find file 'C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Test_Framework\Test_LoginToUniFi.xaml'._x000D_
-File name: 'C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Test_Framework\Test_LoginToUniFi.xaml'_x000D_
-   at System.IO.__Error.WinIOError(Int32 errorCode, String maybeFullPath)_x000D_
-   at System.IO.FileStream.Init(String path, FileMode mode, FileAccess access, Int32 rights, Boolean useRights, FileShare share, Int32 bufferSize, FileOptions options, SECURITY_ATTRIBUTES secAttrs, String msgPath, Boolean bFromProxy, Boolean useLongPath, Boolean checkHost)_x000D_
-   at System.IO.FileStream..ctor(String path, FileMode mode, FileAccess access, FileShare share)_x000D_
-   at UiPath.Executor.WorkflowRuntime.GetWorkflowFileStream(String workflowFile) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 87_x000D_
-   at UiPath.Executor.WorkflowRuntime.Load(String workflowFile) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 74_x000D_
-   at UiPath.Executor.WorkflowRunner.BeginExecuteInProcess(AsyncCallback callback, TaskCompletionSource`1 taskCompletionSource) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 240_x000D_
-   at UiPath.Executor.WorkflowRunner.BeginExecute(AsyncCallback callback, Object state) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 184_x000D_
-   at UiPath.Core.Activities.InvokeWorkflowFile.BeginExecute(AsyncCodeActivityContext context, AsyncCallback callback, Object state)_x000D_
-   at System.Activities.AsyncCodeActivity.InternalExecute(ActivityInstance instance, ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
-   at System.Activities.ActivityInstance.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
-   at System.Activities.Runtime.ActivityExecutor.ExecuteActivityWorkItem.ExecuteBody(ActivityExecutor executor, BookmarkManager bookmarkManager, Location resultLocation)</t>
-  </si>
-  <si>
-    <t>Should throw AppEx: System.IO.FileNotFoundException: Could not find file 'C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Test_Framework\Test_NavToMenuItem.xaml'._x000D_
-File name: 'C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Test_Framework\Test_NavToMenuItem.xaml'_x000D_
-   at System.IO.__Error.WinIOError(Int32 errorCode, String maybeFullPath)_x000D_
-   at System.IO.FileStream.Init(String path, FileMode mode, FileAccess access, Int32 rights, Boolean useRights, FileShare share, Int32 bufferSize, FileOptions options, SECURITY_ATTRIBUTES secAttrs, String msgPath, Boolean bFromProxy, Boolean useLongPath, Boolean checkHost)_x000D_
-   at System.IO.FileStream..ctor(String path, FileMode mode, FileAccess access, FileShare share)_x000D_
-   at UiPath.Executor.WorkflowRuntime.GetWorkflowFileStream(String workflowFile) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 87_x000D_
-   at UiPath.Executor.WorkflowRuntime.Load(String workflowFile) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 74_x000D_
-   at UiPath.Executor.WorkflowRunner.BeginExecuteInProcess(AsyncCallback callback, TaskCompletionSource`1 taskCompletionSource) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 240_x000D_
-   at UiPath.Executor.WorkflowRunner.BeginExecute(AsyncCallback callback, Object state) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 184_x000D_
-   at UiPath.Core.Activities.InvokeWorkflowFile.BeginExecute(AsyncCodeActivityContext context, AsyncCallback callback, Object state)_x000D_
-   at System.Activities.AsyncCodeActivity.InternalExecute(ActivityInstance instance, ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
-   at System.Activities.ActivityInstance.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
-   at System.Activities.Runtime.ActivityExecutor.ExecuteActivityWorkItem.ExecuteBody(ActivityExecutor executor, BookmarkManager bookmarkManager, Location resultLocation)</t>
-  </si>
-  <si>
-    <t>Wasn't meant to throw AppEx: System.IO.FileNotFoundException: Could not find file 'C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Test_Framework\Test_NavToMenuItem.xaml'._x000D_
-File name: 'C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Test_Framework\Test_NavToMenuItem.xaml'_x000D_
-   at System.IO.__Error.WinIOError(Int32 errorCode, String maybeFullPath)_x000D_
-   at System.IO.FileStream.Init(String path, FileMode mode, FileAccess access, Int32 rights, Boolean useRights, FileShare share, Int32 bufferSize, FileOptions options, SECURITY_ATTRIBUTES secAttrs, String msgPath, Boolean bFromProxy, Boolean useLongPath, Boolean checkHost)_x000D_
-   at System.IO.FileStream..ctor(String path, FileMode mode, FileAccess access, FileShare share)_x000D_
-   at UiPath.Executor.WorkflowRuntime.GetWorkflowFileStream(String workflowFile) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 87_x000D_
-   at UiPath.Executor.WorkflowRuntime.Load(String workflowFile) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 74_x000D_
-   at UiPath.Executor.WorkflowRunner.BeginExecuteInProcess(AsyncCallback callback, TaskCompletionSource`1 taskCompletionSource) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 240_x000D_
-   at UiPath.Executor.WorkflowRunner.BeginExecute(AsyncCallback callback, Object state) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 184_x000D_
-   at UiPath.Core.Activities.InvokeWorkflowFile.BeginExecute(AsyncCodeActivityContext context, AsyncCallback callback, Object state)_x000D_
-   at System.Activities.AsyncCodeActivity.InternalExecute(ActivityInstance instance, ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
-   at System.Activities.ActivityInstance.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
-   at System.Activities.Runtime.ActivityExecutor.ExecuteActivityWorkItem.ExecuteBody(ActivityExecutor executor, BookmarkManager bookmarkManager, Location resultLocation)</t>
   </si>
   <si>
     <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: RM Number ---&gt; UiPath.Core.Activities.ActivityTimeoutException: Activity timeout exceeded_x000D_
@@ -360,79 +312,142 @@
    at System.Activities.Runtime.BookmarkCallbackWrapper.Invoke(NativeActivityContext context, Bookmark bookmark, Object value)_x000D_
    at System.Activities.Runtime.BookmarkWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
    --- End of inner exception stack trace ---_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
   <si>
     <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Op Unit: Faculty, School, Section, Site &amp; Under Acc: Opal, Site, Fund, Function_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
   <si>
     <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Op Unit: Faculty_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
   <si>
     <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Op Unit: School_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
   <si>
     <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Op Unit: Section_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
   <si>
     <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Op Unit: Site_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
   <si>
     <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Under Acc: Opal_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
   <si>
     <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Under Acc: Site_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
   <si>
     <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Under Acc: Fund_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
   <si>
     <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: Under Acc: Function_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in d:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Test_Framework\Unifi\Test_SearchRMNumber.xaml</t>
+  </si>
+  <si>
+    <t>Wasn't meant to throw BRE: System.Activities.Statements.WorkflowTerminatedException: 10.2-11.3	No Updated Entries_x000D_
+I wasn't able to update global as the rows were: Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Cancelled, Done, Done, Done, Done, Cancelled, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Cancelled, Cancelled, Done, Done, Done, Done, Done, Done, Cancelled, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Cancelled, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Wasn't meant to throw BRE: System.Activities.Statements.WorkflowTerminatedException: No matching values were found._x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: 10.2-11.3	No Updated Entries_x000D_
+I wasn't able to update 201100215 as the rows were: Done, Cancelled, Cancelled, Done, Done, Done_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Test_Framework\Unifi\Test_NavToMenuItem.xaml</t>
+  </si>
+  <si>
+    <t>Test_Framework\Unifi\Test_LoginToUniFi.xaml</t>
+  </si>
+  <si>
+    <t>\Test_Framework\Unifi\Test_LoginToUniFi.xaml</t>
+  </si>
+  <si>
+    <t>Should throw AppEx: UiPath.Core.SelectorNotFoundException: Cannot find the UI element corresponding to this selector: &lt;webctrl tag='UL' parentclass='pthnavscroll' /&gt;&lt;webctrl tag='A' aaname='Invalid Selection' /&gt; ---&gt; System.Runtime.InteropServices.COMException: Cannot find the UI element corresponding to this selector: &lt;webctrl tag='UL' parentclass='pthnavscroll' /&gt;&lt;webctrl tag='A' aaname='Invalid Selection' /&gt;_x000D_
+   at UiPath.UiNodeClass.FindFirst(UiFindScope scope, String nodeID)_x000D_
+   at UiPath.Core.UiElement.FindFirst(FindScope scope, Selector selector)_x000D_
+   --- End of inner exception stack trace ---_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>\Test_Framework\FileServing\Test_MountFileServer.xaml</t>
+  </si>
+  <si>
+    <t>\Test_Framework\FileServing\Test_UnmountAllDrives.xaml</t>
+  </si>
+  <si>
+    <t>\Test_Framework\FileServing\Test_UnmountFileServer.xaml</t>
+  </si>
+  <si>
+    <t>\Test_Framework\Unifi\Test_UpdateRMProposal.xaml</t>
+  </si>
+  <si>
+    <t>\Test_Framework\Unifi\Test_LogoutUniFi.xaml</t>
+  </si>
+  <si>
+    <t>Test_Framework\Exchange\Test_ScrapeEmail_ValidateData.xaml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -784,22 +799,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -816,7 +831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -825,58 +840,58 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -885,426 +900,453 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="8">
+        <v>2018001377</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="8">
-        <v>2018001377</v>
-      </c>
-      <c r="E24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="8" t="s">
+      <c r="D35" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E35" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="10" t="s">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="10" t="s">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E37" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" t="s">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="10"/>
+      <c r="E38" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" t="s">
-        <v>58</v>
-      </c>
-      <c r="E33" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>80</v>
-      </c>
-      <c r="B34" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" t="s">
-        <v>60</v>
-      </c>
-      <c r="E35" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" t="s">
-        <v>61</v>
-      </c>
-      <c r="E36" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>80</v>
-      </c>
-      <c r="B37" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" t="s">
-        <v>62</v>
-      </c>
-      <c r="E37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" t="s">
-        <v>63</v>
-      </c>
-      <c r="E38" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="D39" s="10"/>
+    </row>
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" t="s">
-        <v>65</v>
-      </c>
-      <c r="E40" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D41"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D42"/>
+        <v>107</v>
+      </c>
+      <c r="D40" s="10"/>
+    </row>
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:B20 B2:B13 B23:B40" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B13 B29:B40 B17:B27">
       <formula1>"Success,BRE,AppEx"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1314,16 +1356,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="32.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -1356,24 +1398,24 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>6</v>
@@ -1381,27 +1423,27 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>7</v>
@@ -1415,13 +1457,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1430,48 +1472,48 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10"/>
       <c r="D10" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>10</v>
@@ -1479,423 +1521,465 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C17" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="D17" s="5" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="5">
-        <v>2018001377</v>
+        <v>21</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="5">
-        <v>200000199</v>
+        <v>21</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="5">
-        <v>2018001812</v>
+        <v>21</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>19</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="5">
-        <v>201100215</v>
+      <c r="C27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E34" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="B35" s="2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>60</v>
+        <v>77</v>
+      </c>
+      <c r="D35" s="5">
+        <v>2018001377</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>61</v>
+        <v>79</v>
+      </c>
+      <c r="D36" s="5">
+        <v>200000199</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="5">
+        <v>2018001812</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="5">
+        <v>201100215</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>101</v>
+    </row>
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:D1"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B30" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B30">
       <formula1>"Success,BRE,AppEx"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
ScrapeEmail.xaml added trimming whitespace off RM number and check if value is blank SearchRMNumber.xaml now uses EnterValue.xaml workflow for typing the rm number
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Test_Framework/_Tests.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Test_Framework/_Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="108">
   <si>
     <t>WorkflowFile</t>
   </si>
@@ -372,19 +372,6 @@
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
   </si>
   <si>
-    <t>Should throw BRE: System.Activities.Statements.WorkflowTerminatedException: 7.1	Invalid RM Number_x000D_
-The RM number is missing or the email is not a proforma template ---&gt; System.Activities.Statements.WorkflowTerminatedException: Op Unit: Faculty, School, Section, Site &amp; Under Acc: Opal, Site, Fund, Function_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
-   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
-   --- End of inner exception stack trace ---_x000D_
-   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
-   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
-   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
-  </si>
-  <si>
     <t>Should throw AppEx: UiPath.Core.SelectorNotFoundException: Cannot find the UI element corresponding to this selector: &lt;webctrl tag='UL' parentclass='pthnavscroll' /&gt;&lt;webctrl tag='A' aaname='Invalid Selection' /&gt; ---&gt; System.Runtime.InteropServices.COMException: Cannot find the UI element corresponding to this selector: &lt;webctrl tag='UL' parentclass='pthnavscroll' /&gt;&lt;webctrl tag='A' aaname='Invalid Selection' /&gt;_x000D_
    at UiPath.UiNodeClass.FindFirst(UiFindScope scope, String nodeID)_x000D_
    at UiPath.Core.UiElement.FindFirst(FindScope scope, Selector selector, IVariableResolver resolver)_x000D_
@@ -397,6 +384,110 @@
   <si>
     <t>Wasn't meant to throw BRE: System.Activities.Statements.WorkflowTerminatedException: 10.2-11.3	No Updated Entries_x000D_
 I wasn't able to update  as the rows were: Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Cancelled, Done, Done, Done, Done, Cancelled, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Cancelled, Cancelled, Done, Done, Done, Done, Done, Done, Cancelled, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done, Cancelled, Done, Done, Done, Done, Done, Done, Done, Done, Done, Done_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Wasn't meant to throw BRE: System.Activities.Statements.WorkflowTerminatedException: 7.1	Invalid RM Number_x000D_
+The RM number is missing or the email is not a proforma template ---&gt; System.Activities.Statements.WorkflowTerminatedException: Op Unit: Faculty_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   --- End of inner exception stack trace ---_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Wasn't meant to throw BRE: System.Activities.Statements.WorkflowTerminatedException: 7.1	Invalid RM Number_x000D_
+The RM number is missing or the email is not a proforma template ---&gt; System.Activities.Statements.WorkflowTerminatedException: Op Unit: School_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   --- End of inner exception stack trace ---_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Wasn't meant to throw BRE: System.Activities.Statements.WorkflowTerminatedException: 7.1	Invalid RM Number_x000D_
+The RM number is missing or the email is not a proforma template ---&gt; System.Activities.Statements.WorkflowTerminatedException: Op Unit: Section_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   --- End of inner exception stack trace ---_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Wasn't meant to throw BRE: System.Activities.Statements.WorkflowTerminatedException: 7.1	Invalid RM Number_x000D_
+The RM number is missing or the email is not a proforma template ---&gt; System.Activities.Statements.WorkflowTerminatedException: Op Unit: Site_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   --- End of inner exception stack trace ---_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Wasn't meant to throw BRE: System.Activities.Statements.WorkflowTerminatedException: 7.1	Invalid RM Number_x000D_
+The RM number is missing or the email is not a proforma template ---&gt; System.Activities.Statements.WorkflowTerminatedException: Under Acc: Opal_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   --- End of inner exception stack trace ---_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Wasn't meant to throw BRE: System.Activities.Statements.WorkflowTerminatedException: 7.1	Invalid RM Number_x000D_
+The RM number is missing or the email is not a proforma template ---&gt; System.Activities.Statements.WorkflowTerminatedException: Under Acc: Site_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   --- End of inner exception stack trace ---_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Wasn't meant to throw BRE: System.Activities.Statements.WorkflowTerminatedException: 7.1	Invalid RM Number_x000D_
+The RM number is missing or the email is not a proforma template ---&gt; System.Activities.Statements.WorkflowTerminatedException: Under Acc: Fund_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   --- End of inner exception stack trace ---_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>Wasn't meant to throw BRE: System.Activities.Statements.WorkflowTerminatedException: 7.1	Invalid RM Number_x000D_
+The RM number is missing or the email is not a proforma template ---&gt; System.Activities.Statements.WorkflowTerminatedException: Under Acc: Function_x000D_
+   at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
+   at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
+   at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)_x000D_
+   --- End of inner exception stack trace ---_x000D_
    at UiPath.Executor.WorkflowRunner.EndExecute(IAsyncResult result) in D:\a\1\s\Robot\UiPath.Executor\WorkflowRuntime.cs:line 208_x000D_
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
@@ -761,7 +852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -1324,7 +1415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1484,7 +1575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="390" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1497,11 +1588,11 @@
       <c r="D11" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -1514,7 +1605,7 @@
       <c r="D12" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1560,16 +1651,16 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>52</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>79</v>
       </c>
@@ -1582,11 +1673,11 @@
       <c r="D17" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>79</v>
       </c>
@@ -1599,161 +1690,161 @@
       <c r="D18" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="345" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>98</v>
+      <c r="E27" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1787,7 +1878,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="240" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>72</v>
       </c>
@@ -1800,8 +1891,8 @@
       <c r="D31" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>99</v>
+      <c r="E31" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1821,7 +1912,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>69</v>
       </c>
@@ -1831,8 +1922,8 @@
       <c r="C33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>100</v>
+      <c r="E33" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1852,7 +1943,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>69</v>
       </c>
@@ -1865,7 +1956,7 @@
       <c r="D35" s="5">
         <v>200000199</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="2" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1886,7 +1977,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>69</v>
       </c>
@@ -1899,11 +1990,11 @@
       <c r="D37" s="5">
         <v>201100215</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>69</v>
       </c>
@@ -1913,8 +2004,8 @@
       <c r="C38" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>100</v>
+      <c r="E38" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added ProcessTransaction test, user selects an email from the list and that single transaction is processed
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Test_Framework/_Tests.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Test_Framework/_Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="109">
   <si>
     <t>WorkflowFile</t>
   </si>
@@ -492,6 +492,9 @@
    at UiPath.Core.Activities.InvokeWorkflowFile.EndExecute(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.System.Activities.IAsyncCodeActivity.FinishExecution(AsyncCodeActivityContext context, IAsyncResult result)_x000D_
    at System.Activities.AsyncCodeActivity.CompleteAsyncCodeActivityData.CompleteAsyncCodeActivityWorkItem.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)</t>
+  </si>
+  <si>
+    <t>SSO_rpa00002,https://fs92fnta.dev.unifi.uq.edu.au/psp/ps/?cmd=login</t>
   </si>
 </sst>
 </file>
@@ -1415,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,7 +1875,7 @@
         <v>63</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>64</v>

</xml_diff>